<commit_message>
Bunch of changes.. sry
</commit_message>
<xml_diff>
--- a/work_reference.xlsx
+++ b/work_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oskari\Documents\BodyCount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836E75AF-259D-4173-9B6F-A7411B04BCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989E9C0C-F3A9-4932-B97E-0C7E2274E591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3540" windowWidth="38610" windowHeight="15345" xr2:uid="{C175BA65-C788-4E3B-AACC-D273C035F0F3}"/>
+    <workbookView xWindow="58635" yWindow="3135" windowWidth="27030" windowHeight="15345" xr2:uid="{C175BA65-C788-4E3B-AACC-D273C035F0F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-[$DKK]\ * #,##0.00_-;\-[$DKK]\ * #,##0.00_-;_-[$DKK]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$DKK]\ * #,##0.00_-;\-[$DKK]\ * #,##0.00_-;_-[$DKK]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -99,10 +99,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +420,7 @@
   <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>250</v>
       </c>
       <c r="F2" t="s">
@@ -462,9 +462,9 @@
       </c>
       <c r="C3" s="1">
         <f>SUM(I:I)</f>
-        <v>0.39236111111111116</v>
-      </c>
-      <c r="F3" s="2">
+        <v>0.66319444444444442</v>
+      </c>
+      <c r="F3" s="3">
         <v>45602</v>
       </c>
       <c r="G3" s="1">
@@ -482,11 +482,11 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <f>C3*24*C2</f>
-        <v>2354.166666666667</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>3979.1666666666665</v>
+      </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="1">
         <v>0.85416666666666663</v>
       </c>
@@ -494,7 +494,7 @@
         <v>0.94444444444444442</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I6" si="0">H4-G4</f>
+        <f t="shared" ref="I4:I10" si="0">H4-G4</f>
         <v>9.027777777777779E-2</v>
       </c>
     </row>
@@ -502,11 +502,11 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <f>C4*0.68</f>
-        <v>1600.8333333333337</v>
-      </c>
-      <c r="F5" s="2">
+        <v>2705.8333333333335</v>
+      </c>
+      <c r="F5" s="3">
         <v>45605</v>
       </c>
       <c r="G5" s="1">
@@ -521,7 +521,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F6" s="2"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="1">
         <v>0.875</v>
       </c>
@@ -533,16 +533,70 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="3">
+        <v>45606</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+      <c r="G8" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="F9" s="3">
+        <v>45613</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.9375</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Match top level occurences as groups
</commit_message>
<xml_diff>
--- a/work_reference.xlsx
+++ b/work_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oskari\Documents\BodyCount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989E9C0C-F3A9-4932-B97E-0C7E2274E591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CE4C51-60FE-443C-B540-D8A85C653146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58635" yWindow="3135" windowWidth="27030" windowHeight="15345" xr2:uid="{C175BA65-C788-4E3B-AACC-D273C035F0F3}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C175BA65-C788-4E3B-AACC-D273C035F0F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,13 +96,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00CAE36-1E69-4377-8A1B-200D917D115F}">
-  <dimension ref="B1:I10"/>
+  <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +463,7 @@
       </c>
       <c r="C3" s="1">
         <f>SUM(I:I)</f>
-        <v>0.66319444444444442</v>
+        <v>0.18402777777777773</v>
       </c>
       <c r="F3" s="3">
         <v>45602</v>
@@ -484,7 +485,7 @@
       </c>
       <c r="C4" s="2">
         <f>C3*24*C2</f>
-        <v>3979.1666666666665</v>
+        <v>1104.1666666666665</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="1">
@@ -494,7 +495,7 @@
         <v>0.94444444444444442</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I10" si="0">H4-G4</f>
+        <f t="shared" ref="I4:I11" si="0">H4-G4</f>
         <v>9.027777777777779E-2</v>
       </c>
     </row>
@@ -504,7 +505,7 @@
       </c>
       <c r="C5" s="2">
         <f>C4*0.68</f>
-        <v>2705.8333333333335</v>
+        <v>750.83333333333326</v>
       </c>
       <c r="F5" s="3">
         <v>45605</v>
@@ -589,6 +590,18 @@
       <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>0.10416666666666663</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="4">
+        <v>45626</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.47916666666666669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>